<commit_message>
[ add] example 1.4
</commit_message>
<xml_diff>
--- a/Ex01/scheduling.xlsx
+++ b/Ex01/scheduling.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pchulla\Documents\Betagro\Gurobipy-optimization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pchulla\Documents\Betagro\Gurobipy-optimization\Ex01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C96C6D-327B-4843-A6CB-6920DD49D3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BB408E-7ED3-4F78-88FC-6C24220B23A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -657,7 +657,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1579,7 +1579,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1623,7 +1623,7 @@
         <v>45</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>15</v>
@@ -1646,7 +1646,7 @@
         <v>46</v>
       </c>
       <c r="C3">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>15</v>
@@ -1669,7 +1669,7 @@
         <v>47</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>15</v>
@@ -1692,7 +1692,7 @@
         <v>48</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>15</v>
@@ -1715,7 +1715,7 @@
         <v>49</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>15</v>
@@ -1738,7 +1738,7 @@
         <v>50</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>15</v>
@@ -1761,7 +1761,7 @@
         <v>51</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>15</v>
@@ -1784,7 +1784,7 @@
         <v>52</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>15</v>
@@ -1807,7 +1807,7 @@
         <v>53</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>15</v>
@@ -1830,7 +1830,7 @@
         <v>54</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>15</v>
@@ -1853,7 +1853,7 @@
         <v>55</v>
       </c>
       <c r="C12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <v>15</v>
@@ -1876,7 +1876,7 @@
         <v>56</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <v>15</v>

</xml_diff>